<commit_message>
Changed views and add Excel
</commit_message>
<xml_diff>
--- a/Excel_reports/Summary_DPD.xlsx
+++ b/Excel_reports/Summary_DPD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studia\Test_project\DE---Project\Excel_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61CDAB24-8054-4591-BB6B-F3E8FB28DEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707EB03E-9337-4F7E-B802-01FC8DDE8865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6315" yWindow="3180" windowWidth="38700" windowHeight="15345" xr2:uid="{29BEB99F-D14C-4624-835A-F88BB8B01CD0}"/>
+    <workbookView xWindow="5970" yWindow="2835" windowWidth="38700" windowHeight="15345" xr2:uid="{29BEB99F-D14C-4624-835A-F88BB8B01CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="DPD_bucket_report" sheetId="2" r:id="rId1"/>
@@ -289,7 +289,7 @@
               <c:f>DPD_bucket_report!$A$2:$A$83</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>40209</c:v>
                 </c:pt>
@@ -315,37 +315,40 @@
                   <c:v>40421</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>40451</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>40482</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>40512</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
+                  <c:v>40543</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>40574</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>40602</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
                   <c:v>40633</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="15">
                   <c:v>40663</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
                   <c:v>40694</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="17">
                   <c:v>40724</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="18">
                   <c:v>40755</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="19">
                   <c:v>40786</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>40816</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -355,63 +358,66 @@
               <c:f>DPD_bucket_report!$C$2:$C$83</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1734</c:v>
+                  <c:v>6291</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1419</c:v>
+                  <c:v>12228</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2995</c:v>
+                  <c:v>29122</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4031</c:v>
+                  <c:v>46115</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14618</c:v>
+                  <c:v>59532</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3955</c:v>
+                  <c:v>84605</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8229</c:v>
+                  <c:v>107300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12150</c:v>
+                  <c:v>130470</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22783</c:v>
+                  <c:v>165181</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8658</c:v>
+                  <c:v>180795</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10350</c:v>
+                  <c:v>209209</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11711</c:v>
+                  <c:v>228955</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21568</c:v>
+                  <c:v>238576</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40258</c:v>
+                  <c:v>269787</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10814</c:v>
+                  <c:v>280518</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13415</c:v>
+                  <c:v>274371</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3349</c:v>
+                  <c:v>294721</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>16955</c:v>
+                  <c:v>313756</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>383041</c:v>
+                  <c:v>343281</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>352441</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -543,7 +549,7 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>m/d/yyyy</c:formatCode>
-                      <c:ptCount val="19"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
                         <c:v>40209</c:v>
                       </c:pt>
@@ -569,37 +575,40 @@
                         <c:v>40421</c:v>
                       </c:pt>
                       <c:pt idx="8">
+                        <c:v>40451</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
                         <c:v>40482</c:v>
                       </c:pt>
-                      <c:pt idx="9">
+                      <c:pt idx="10">
                         <c:v>40512</c:v>
                       </c:pt>
-                      <c:pt idx="10">
+                      <c:pt idx="11">
+                        <c:v>40543</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
                         <c:v>40574</c:v>
                       </c:pt>
-                      <c:pt idx="11">
+                      <c:pt idx="13">
                         <c:v>40602</c:v>
                       </c:pt>
-                      <c:pt idx="12">
+                      <c:pt idx="14">
                         <c:v>40633</c:v>
                       </c:pt>
-                      <c:pt idx="13">
+                      <c:pt idx="15">
                         <c:v>40663</c:v>
                       </c:pt>
-                      <c:pt idx="14">
+                      <c:pt idx="16">
                         <c:v>40694</c:v>
                       </c:pt>
-                      <c:pt idx="15">
+                      <c:pt idx="17">
                         <c:v>40724</c:v>
                       </c:pt>
-                      <c:pt idx="16">
+                      <c:pt idx="18">
                         <c:v>40755</c:v>
                       </c:pt>
-                      <c:pt idx="17">
+                      <c:pt idx="19">
                         <c:v>40786</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>40816</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -615,63 +624,66 @@
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="19"/>
+                      <c:ptCount val="20"/>
                       <c:pt idx="0">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>2</c:v>
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>3</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4064,17 +4076,17 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>82</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="DPD_BUCKET">
@@ -4097,7 +4109,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -4300,7 +4312,7 @@
   <autoFilter ref="A1:C83" xr:uid="{C41816E6-F9FE-4765-996F-2B3A03A079A5}">
     <filterColumn colId="1">
       <filters>
-        <filter val="2"/>
+        <filter val="3"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4626,7 +4638,7 @@
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y59" sqref="Y59"/>
+      <selection activeCell="T67" sqref="T67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5120,7 +5132,7 @@
         <v>413949</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>40209</v>
       </c>
@@ -5131,7 +5143,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>40237</v>
       </c>
@@ -5142,7 +5154,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>40268</v>
       </c>
@@ -5153,7 +5165,7 @@
         <v>2995</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>40298</v>
       </c>
@@ -5164,7 +5176,7 @@
         <v>4031</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>40329</v>
       </c>
@@ -5175,7 +5187,7 @@
         <v>14618</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>40359</v>
       </c>
@@ -5186,7 +5198,7 @@
         <v>3955</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>40390</v>
       </c>
@@ -5197,7 +5209,7 @@
         <v>8229</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>40421</v>
       </c>
@@ -5208,7 +5220,7 @@
         <v>12150</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>40482</v>
       </c>
@@ -5219,7 +5231,7 @@
         <v>22783</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>40512</v>
       </c>
@@ -5230,7 +5242,7 @@
         <v>8658</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>40574</v>
       </c>
@@ -5241,7 +5253,7 @@
         <v>10350</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>40602</v>
       </c>
@@ -5252,7 +5264,7 @@
         <v>11711</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>40633</v>
       </c>
@@ -5263,7 +5275,7 @@
         <v>21568</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>40663</v>
       </c>
@@ -5274,7 +5286,7 @@
         <v>40258</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>40694</v>
       </c>
@@ -5285,7 +5297,7 @@
         <v>10814</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>40724</v>
       </c>
@@ -5296,7 +5308,7 @@
         <v>13415</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>40755</v>
       </c>
@@ -5307,7 +5319,7 @@
         <v>3349</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>40786</v>
       </c>
@@ -5318,7 +5330,7 @@
         <v>16955</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>40816</v>
       </c>
@@ -5329,7 +5341,7 @@
         <v>383041</v>
       </c>
     </row>
-    <row r="64" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>40209</v>
       </c>
@@ -5340,7 +5352,7 @@
         <v>6291</v>
       </c>
     </row>
-    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>40237</v>
       </c>
@@ -5351,7 +5363,7 @@
         <v>12228</v>
       </c>
     </row>
-    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>40268</v>
       </c>
@@ -5362,7 +5374,7 @@
         <v>29122</v>
       </c>
     </row>
-    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>40298</v>
       </c>
@@ -5373,7 +5385,7 @@
         <v>46115</v>
       </c>
     </row>
-    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>40329</v>
       </c>
@@ -5384,7 +5396,7 @@
         <v>59532</v>
       </c>
     </row>
-    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>40359</v>
       </c>
@@ -5395,7 +5407,7 @@
         <v>84605</v>
       </c>
     </row>
-    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>40390</v>
       </c>
@@ -5406,7 +5418,7 @@
         <v>107300</v>
       </c>
     </row>
-    <row r="71" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>40421</v>
       </c>
@@ -5417,7 +5429,7 @@
         <v>130470</v>
       </c>
     </row>
-    <row r="72" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>40451</v>
       </c>
@@ -5428,7 +5440,7 @@
         <v>165181</v>
       </c>
     </row>
-    <row r="73" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>40482</v>
       </c>
@@ -5439,7 +5451,7 @@
         <v>180795</v>
       </c>
     </row>
-    <row r="74" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>40512</v>
       </c>
@@ -5450,7 +5462,7 @@
         <v>209209</v>
       </c>
     </row>
-    <row r="75" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>40543</v>
       </c>
@@ -5461,7 +5473,7 @@
         <v>228955</v>
       </c>
     </row>
-    <row r="76" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>40574</v>
       </c>
@@ -5472,7 +5484,7 @@
         <v>238576</v>
       </c>
     </row>
-    <row r="77" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>40602</v>
       </c>
@@ -5483,7 +5495,7 @@
         <v>269787</v>
       </c>
     </row>
-    <row r="78" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>40633</v>
       </c>
@@ -5494,7 +5506,7 @@
         <v>280518</v>
       </c>
     </row>
-    <row r="79" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>40663</v>
       </c>
@@ -5505,7 +5517,7 @@
         <v>274371</v>
       </c>
     </row>
-    <row r="80" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>40694</v>
       </c>
@@ -5516,7 +5528,7 @@
         <v>294721</v>
       </c>
     </row>
-    <row r="81" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>40724</v>
       </c>
@@ -5527,7 +5539,7 @@
         <v>313756</v>
       </c>
     </row>
-    <row r="82" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>40755</v>
       </c>
@@ -5538,7 +5550,7 @@
         <v>343281</v>
       </c>
     </row>
-    <row r="83" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>40786</v>
       </c>

</xml_diff>